<commit_message>
Partial fill out of QL form
</commit_message>
<xml_diff>
--- a/doc/QLFeatures_Table_Template.xlsx
+++ b/doc/QLFeatures_Table_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Judith Michael\Documents\Publikationen\_SVNpaper\trunk\xx.LanguageWorkbenchComparison\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\digitalgardeners\repo\mps-lwc25\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D74C18-DB67-41E3-A593-1FC6C0DEF685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11AFC3A-BEA7-4396-9842-C6FA0647D631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="2160" windowWidth="16845" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
   <si>
     <t>Syntax</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Feature</t>
   </si>
   <si>
-    <t>Language Workbench Name</t>
-  </si>
-  <si>
     <t>fully implemented</t>
   </si>
   <si>
@@ -112,6 +109,15 @@
   </si>
   <si>
     <t>Please add a comment in this case what partially means</t>
+  </si>
+  <si>
+    <t>JetBrains MPS</t>
+  </si>
+  <si>
+    <t>partially implemented/limited support</t>
+  </si>
+  <si>
+    <t>was asked not to implement as part of assignment</t>
   </si>
 </sst>
 </file>
@@ -244,10 +250,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -258,7 +263,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -538,11 +543,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
@@ -552,77 +557,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>25</v>
+      <c r="B1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="E3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="6"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="E3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
       <c r="C4" s="1"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="8"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
       <c r="C5" s="1"/>
-      <c r="E5" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="8"/>
+      <c r="E5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
       <c r="C6" s="1"/>
-      <c r="E6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>28</v>
+      <c r="E6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="E7" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="10"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="E7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -635,8 +648,13 @@
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
       <c r="C9" s="1"/>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -644,26 +662,35 @@
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="2"/>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -677,57 +704,81 @@
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="1"/>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>